<commit_message>
Changed the Leave Apply functionality based on the Holiday
</commit_message>
<xml_diff>
--- a/frontend/src/assets/samplesheet/holidaysamplesheet.xlsx
+++ b/frontend/src/assets/samplesheet/holidaysamplesheet.xlsx
@@ -34,6 +34,9 @@
     <t>Repeat</t>
   </si>
   <si>
+    <t>Leavefor</t>
+  </si>
+  <si>
     <t>May Day</t>
   </si>
   <si>
@@ -43,7 +46,13 @@
     <t>National Worker's Day</t>
   </si>
   <si>
+    <t>Night Shift</t>
+  </si>
+  <si>
     <t>Diwali</t>
+  </si>
+  <si>
+    <t>Day Shift</t>
   </si>
 </sst>
 </file>
@@ -375,7 +384,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -403,22 +412,28 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
         <v>45778</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -426,16 +441,19 @@
         <v>45935</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>